<commit_message>
enhance Labmanagement for dynamic html
</commit_message>
<xml_diff>
--- a/microblog/app/Uploads/data.xlsx
+++ b/microblog/app/Uploads/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="6990"/>
@@ -32,10 +32,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="A41" authorId="0">
+    <comment ref="A41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A45" authorId="0">
+    <comment ref="A45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -83,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C45" authorId="0">
+    <comment ref="C45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -615,7 +615,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -633,7 +633,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -654,7 +654,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -675,7 +675,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -696,7 +696,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -729,7 +729,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1809,7 +1809,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1821,7 +1821,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1846,7 +1846,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1857,7 +1857,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2339,7 +2339,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2349,7 +2349,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2369,7 +2369,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2390,7 +2390,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2409,7 +2409,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2423,7 +2423,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2433,7 +2433,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3139,15 +3139,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="176" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3162,21 +3162,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3191,7 +3191,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3225,7 +3225,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3243,7 +3243,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3269,7 +3269,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3300,7 +3300,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3308,7 +3308,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3344,6 +3344,13 @@
       <color rgb="FFA6A6A6"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="23">
@@ -3685,7 +3692,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3847,10 +3854,10 @@
     <xf numFmtId="0" fontId="20" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="21" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="21" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="21" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4012,12 +4019,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="差" xfId="2" builtinId="27"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -4047,7 +4055,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4089,7 +4097,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4122,9 +4130,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4157,6 +4182,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4339,998 +4381,1000 @@
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" style="125" customWidth="1"/>
+    <col min="2" max="2" width="17.25" style="125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" style="125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9" style="125"/>
+    <col min="6" max="6" width="15.625" style="125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.75" style="125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.25" style="125" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="125" t="s">
         <v>301</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="125" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="125" t="s">
         <v>302</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="125" t="s">
         <v>303</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="125" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="125" t="s">
         <v>305</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="125" t="s">
         <v>303</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="125" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="125" t="s">
         <v>97</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="125" t="s">
         <v>306</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="125" t="s">
         <v>98</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="125" t="s">
         <v>99</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="125" t="s">
         <v>100</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="125" t="s">
         <v>303</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="125" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="125" customFormat="1">
-      <c r="A5" s="125" t="s">
+    <row r="5" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="126" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="126" t="s">
         <v>307</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="126" t="s">
         <v>308</v>
       </c>
-      <c r="D5" s="125" t="s">
+      <c r="D5" s="126" t="s">
         <v>309</v>
       </c>
-      <c r="E5" s="125" t="s">
+      <c r="E5" s="126" t="s">
         <v>310</v>
       </c>
-      <c r="F5" s="125" t="s">
+      <c r="F5" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="125" t="s">
+      <c r="G5" s="126" t="s">
         <v>311</v>
       </c>
-      <c r="H5" s="125" t="s">
+      <c r="H5" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="125" customFormat="1">
-      <c r="A6" s="125" t="s">
+    <row r="6" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="126" t="s">
         <v>307</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="125" t="s">
+      <c r="E6" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="125" t="s">
+      <c r="G6" s="126" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="125" t="s">
+      <c r="H6" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="125" t="s">
         <v>307</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="125" t="s">
         <v>312</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="125" t="s">
         <v>307</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="125" t="s">
         <v>313</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="125" t="s">
         <v>314</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="125" t="s">
         <v>315</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="125" customFormat="1">
-      <c r="A9" s="125" t="s">
+    <row r="9" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="125" t="s">
+      <c r="B9" s="126" t="s">
         <v>316</v>
       </c>
-      <c r="C9" s="125" t="s">
+      <c r="C9" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="125" t="s">
+      <c r="D9" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="125" t="s">
+      <c r="E9" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="125" t="s">
+      <c r="F9" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="125" t="s">
+      <c r="G9" s="126" t="s">
         <v>317</v>
       </c>
-      <c r="H9" s="125" t="s">
+      <c r="H9" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="125" customFormat="1">
-      <c r="A10" s="125" t="s">
+    <row r="10" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="126" t="s">
         <v>318</v>
       </c>
-      <c r="B10" s="125" t="s">
+      <c r="B10" s="126" t="s">
         <v>316</v>
       </c>
-      <c r="C10" s="125" t="s">
+      <c r="C10" s="126" t="s">
         <v>319</v>
       </c>
-      <c r="D10" s="125" t="s">
+      <c r="D10" s="126" t="s">
         <v>320</v>
       </c>
-      <c r="E10" s="125" t="s">
+      <c r="E10" s="126" t="s">
         <v>321</v>
       </c>
-      <c r="F10" s="125" t="s">
+      <c r="F10" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="125" t="s">
+      <c r="G10" s="126" t="s">
         <v>317</v>
       </c>
-      <c r="H10" s="125" t="s">
+      <c r="H10" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="125" customFormat="1">
-      <c r="A11" s="125" t="s">
+    <row r="11" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="126" t="s">
         <v>322</v>
       </c>
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="126" t="s">
         <v>323</v>
       </c>
-      <c r="C11" s="125" t="s">
+      <c r="C11" s="126" t="s">
         <v>324</v>
       </c>
-      <c r="D11" s="125" t="s">
+      <c r="D11" s="126" t="s">
         <v>325</v>
       </c>
-      <c r="E11" s="125" t="s">
+      <c r="E11" s="126" t="s">
         <v>326</v>
       </c>
-      <c r="F11" s="125" t="s">
+      <c r="F11" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="125" t="s">
+      <c r="G11" s="126" t="s">
         <v>327</v>
       </c>
-      <c r="H11" s="125" t="s">
+      <c r="H11" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="125" customFormat="1">
-      <c r="A12" s="125" t="s">
+    <row r="12" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="126" t="s">
         <v>328</v>
       </c>
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="126" t="s">
         <v>323</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="126" t="s">
         <v>329</v>
       </c>
-      <c r="D12" s="125" t="s">
+      <c r="D12" s="126" t="s">
         <v>330</v>
       </c>
-      <c r="E12" s="125" t="s">
+      <c r="E12" s="126" t="s">
         <v>331</v>
       </c>
-      <c r="F12" s="125" t="s">
+      <c r="F12" s="126" t="s">
         <v>303</v>
       </c>
-      <c r="G12" s="125" t="s">
+      <c r="G12" s="126" t="s">
         <v>327</v>
       </c>
-      <c r="H12" s="125" t="s">
+      <c r="H12" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="125" t="s">
         <v>323</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="125" t="s">
         <v>317</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="125" customFormat="1">
-      <c r="A14" s="125" t="s">
+    <row r="14" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="125" t="s">
+      <c r="B14" s="126" t="s">
         <v>316</v>
       </c>
-      <c r="C14" s="125" t="s">
+      <c r="C14" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="125" t="s">
+      <c r="D14" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="125" t="s">
+      <c r="E14" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="125" t="s">
+      <c r="F14" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="125" t="s">
+      <c r="G14" s="126" t="s">
         <v>317</v>
       </c>
-      <c r="H14" s="125" t="s">
+      <c r="H14" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="125" t="s">
         <v>332</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="125" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="125" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="125" customFormat="1">
-      <c r="A16" s="125" t="s">
+    <row r="16" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="125" t="s">
+      <c r="B16" s="126" t="s">
         <v>323</v>
       </c>
-      <c r="C16" s="125" t="s">
+      <c r="C16" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="125" t="s">
+      <c r="D16" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="125" t="s">
+      <c r="E16" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="125" t="s">
+      <c r="F16" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="125" t="s">
+      <c r="G16" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="125" t="s">
+      <c r="H16" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="125" t="s">
         <v>307</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="125" t="s">
         <v>54</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="125" t="s">
         <v>56</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="125" customFormat="1">
-      <c r="A18" s="125" t="s">
+    <row r="18" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="125" t="s">
+      <c r="B18" s="126" t="s">
         <v>307</v>
       </c>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="125" t="s">
+      <c r="D18" s="126" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="125" t="s">
+      <c r="E18" s="126" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="125" t="s">
+      <c r="F18" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="125" t="s">
+      <c r="G18" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="125" t="s">
+      <c r="H18" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="125" t="s">
         <v>332</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="125" t="s">
         <v>56</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="125" t="s">
         <v>333</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="125" t="s">
         <v>316</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="125" t="s">
         <v>334</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="125" t="s">
         <v>335</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="125" t="s">
         <v>336</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="125" customFormat="1">
-      <c r="A21" s="125" t="s">
+    <row r="21" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="126" t="s">
         <v>337</v>
       </c>
-      <c r="B21" s="125" t="s">
+      <c r="B21" s="126" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="125" t="s">
+      <c r="C21" s="126" t="s">
         <v>338</v>
       </c>
-      <c r="D21" s="125" t="s">
+      <c r="D21" s="126" t="s">
         <v>339</v>
       </c>
-      <c r="E21" s="125" t="s">
+      <c r="E21" s="126" t="s">
         <v>340</v>
       </c>
-      <c r="F21" s="125" t="s">
+      <c r="F21" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="125" t="s">
+      <c r="G21" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="125" t="s">
+      <c r="H21" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="125" customFormat="1">
-      <c r="A22" s="125" t="s">
+    <row r="22" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="126" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="125" t="s">
+      <c r="B22" s="126" t="s">
         <v>316</v>
       </c>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="125" t="s">
+      <c r="D22" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="125" t="s">
+      <c r="E22" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="125" t="s">
+      <c r="F22" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="125" t="s">
+      <c r="G22" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="125" t="s">
+      <c r="H22" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="125" t="s">
         <v>341</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="125" t="s">
         <v>316</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="125" t="s">
         <v>342</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="125" t="s">
         <v>343</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="125" t="s">
         <v>344</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="125" t="s">
         <v>311</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="125" t="s">
         <v>345</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="125" t="s">
         <v>316</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="125" t="s">
         <v>346</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="125" t="s">
         <v>347</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="125" t="s">
         <v>348</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="125" t="s">
         <v>317</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="125" t="s">
         <v>349</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="125" t="s">
         <v>323</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="125" t="s">
         <v>350</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="125" t="s">
         <v>351</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="125" t="s">
         <v>352</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="125" t="s">
         <v>317</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="125" t="s">
         <v>353</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="125" t="s">
         <v>323</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="125" t="s">
         <v>354</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="125" t="s">
         <v>355</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="125" t="s">
         <v>356</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="125" t="s">
         <v>317</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="125" customFormat="1">
-      <c r="A27" s="125" t="s">
+    <row r="27" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="126" t="s">
         <v>357</v>
       </c>
-      <c r="B27" s="125" t="s">
+      <c r="B27" s="126" t="s">
         <v>323</v>
       </c>
-      <c r="C27" s="125" t="s">
+      <c r="C27" s="126" t="s">
         <v>358</v>
       </c>
-      <c r="D27" s="125" t="s">
+      <c r="D27" s="126" t="s">
         <v>359</v>
       </c>
-      <c r="E27" s="125" t="s">
+      <c r="E27" s="126" t="s">
         <v>360</v>
       </c>
-      <c r="F27" s="125" t="s">
+      <c r="F27" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="125" t="s">
+      <c r="G27" s="126" t="s">
         <v>317</v>
       </c>
-      <c r="H27" s="125" t="s">
+      <c r="H27" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="125" customFormat="1">
-      <c r="A28" s="125" t="s">
+    <row r="28" spans="1:8" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="126" t="s">
         <v>361</v>
       </c>
-      <c r="B28" s="125" t="s">
+      <c r="B28" s="126" t="s">
         <v>323</v>
       </c>
-      <c r="C28" s="125" t="s">
+      <c r="C28" s="126" t="s">
         <v>362</v>
       </c>
-      <c r="D28" s="125" t="s">
+      <c r="D28" s="126" t="s">
         <v>363</v>
       </c>
-      <c r="E28" s="125" t="s">
+      <c r="E28" s="126" t="s">
         <v>364</v>
       </c>
-      <c r="F28" s="125" t="s">
+      <c r="F28" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="125" t="s">
+      <c r="G28" s="126" t="s">
         <v>317</v>
       </c>
-      <c r="H28" s="125" t="s">
+      <c r="H28" s="126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="125" t="s">
         <v>365</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="125" t="s">
         <v>332</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="125" t="s">
         <v>366</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="125" t="s">
         <v>367</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="125" t="s">
         <v>368</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="125" t="s">
         <v>311</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="125" t="s">
         <v>323</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="125" t="s">
         <v>72</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="125" t="s">
         <v>75</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="125" t="s">
         <v>316</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="125" t="s">
         <v>78</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="125" t="s">
         <v>79</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="125" t="s">
         <v>316</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="125" t="s">
         <v>82</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33" s="125" t="s">
         <v>369</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="125" t="s">
         <v>370</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="125" t="s">
         <v>371</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="125" t="s">
         <v>372</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="125" t="s">
         <v>373</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="125" t="s">
         <v>370</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="125" t="s">
         <v>85</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="125" t="s">
         <v>86</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35" s="125" t="s">
         <v>680</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="125" t="s">
         <v>370</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="125" t="s">
         <v>681</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="125" t="s">
         <v>682</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="125" t="s">
         <v>683</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="125" t="s">
         <v>370</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="125" t="s">
         <v>90</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A37" s="125" t="s">
         <v>92</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="125" t="s">
         <v>370</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="125" t="s">
         <v>93</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="125" t="s">
         <v>94</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="125" t="s">
         <v>95</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="125" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A38" s="125" t="s">
         <v>684</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="125" t="s">
         <v>370</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="125" t="s">
         <v>685</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="125" t="s">
         <v>686</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="125" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5353,18 +5397,18 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.375" customWidth="1"/>
+    <col min="5" max="5" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.25" customWidth="1"/>
     <col min="7" max="7" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>224</v>
       </c>
@@ -5387,7 +5431,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="149.25" customHeight="1">
+    <row r="2" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="61" t="s">
         <v>457</v>
       </c>
@@ -5410,7 +5454,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="409.5">
+    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A3" s="61" t="s">
         <v>463</v>
       </c>
@@ -5433,7 +5477,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="210">
+    <row r="4" spans="1:7" ht="189" x14ac:dyDescent="0.15">
       <c r="A4" s="61" t="s">
         <v>464</v>
       </c>
@@ -5474,13 +5518,13 @@
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="55.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
         <v>485</v>
       </c>
@@ -5491,7 +5535,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="69" t="s">
         <v>487</v>
       </c>
@@ -5502,7 +5546,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24.75">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="71" t="s">
         <v>490</v>
       </c>
@@ -5513,7 +5557,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="108.75" customHeight="1">
+    <row r="4" spans="1:3" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="73" t="s">
         <v>492</v>
       </c>
@@ -5524,7 +5568,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="75" t="s">
         <v>495</v>
       </c>
@@ -5535,7 +5579,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24.75" customHeight="1">
+    <row r="6" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="75" t="s">
         <v>497</v>
       </c>
@@ -5546,7 +5590,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="360" customHeight="1">
+    <row r="7" spans="1:3" ht="360" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="75" t="s">
         <v>250</v>
       </c>
@@ -5557,7 +5601,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="229.5" customHeight="1">
+    <row r="8" spans="1:3" ht="229.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="75" t="s">
         <v>246</v>
       </c>
@@ -5568,7 +5612,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="75" t="s">
         <v>503</v>
       </c>
@@ -5579,7 +5623,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="75" t="s">
         <v>505</v>
       </c>
@@ -5590,7 +5634,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24.75" customHeight="1">
+    <row r="11" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="75" t="s">
         <v>506</v>
       </c>
@@ -5601,7 +5645,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="75" t="s">
         <v>508</v>
       </c>
@@ -5612,7 +5656,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="79" t="s">
         <v>510</v>
       </c>
@@ -5623,7 +5667,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24.75" customHeight="1">
+    <row r="14" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="79" t="s">
         <v>512</v>
       </c>
@@ -5634,7 +5678,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="79" t="s">
         <v>513</v>
       </c>
@@ -5645,7 +5689,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="79" t="s">
         <v>514</v>
       </c>
@@ -5656,7 +5700,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="153">
+    <row r="17" spans="1:3" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A17" s="75" t="s">
         <v>515</v>
       </c>
@@ -5667,7 +5711,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="75" t="s">
         <v>518</v>
       </c>
@@ -5678,7 +5722,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="75" t="s">
         <v>520</v>
       </c>
@@ -5689,7 +5733,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="255" customHeight="1">
+    <row r="20" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="75" t="s">
         <v>522</v>
       </c>
@@ -5700,14 +5744,14 @@
         <v>523</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="75" t="s">
         <v>524</v>
       </c>
       <c r="B21" s="81"/>
       <c r="C21" s="81"/>
     </row>
-    <row r="22" spans="1:3" ht="89.25">
+    <row r="22" spans="1:3" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="83" t="s">
         <v>525</v>
       </c>
@@ -5718,7 +5762,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="409.5" customHeight="1">
+    <row r="23" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="83" t="s">
         <v>528</v>
       </c>
@@ -5729,7 +5773,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="409.5" customHeight="1">
+    <row r="24" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="83" t="s">
         <v>531</v>
       </c>
@@ -5740,7 +5784,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="127.5">
+    <row r="25" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A25" s="79" t="s">
         <v>533</v>
       </c>
@@ -5751,7 +5795,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="79" t="s">
         <v>536</v>
       </c>
@@ -5762,7 +5806,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="409.5" customHeight="1">
+    <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="79" t="s">
         <v>537</v>
       </c>
@@ -5773,7 +5817,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="24.75" customHeight="1">
+    <row r="28" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="84" t="s">
         <v>540</v>
       </c>
@@ -5784,7 +5828,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="89.25" customHeight="1">
+    <row r="29" spans="1:3" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="84" t="s">
         <v>541</v>
       </c>
@@ -5795,7 +5839,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="229.5" customHeight="1">
+    <row r="30" spans="1:3" ht="229.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="84" t="s">
         <v>543</v>
       </c>
@@ -5806,7 +5850,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="242.25">
+    <row r="31" spans="1:3" ht="229.5" x14ac:dyDescent="0.2">
       <c r="A31" s="75" t="s">
         <v>545</v>
       </c>
@@ -5817,7 +5861,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="25.5">
+    <row r="32" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="75" t="s">
         <v>547</v>
       </c>
@@ -5828,7 +5872,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1">
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="75" t="s">
         <v>549</v>
       </c>
@@ -5839,7 +5883,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="36.75">
+    <row r="34" spans="1:3" ht="36" x14ac:dyDescent="0.2">
       <c r="A34" s="75" t="s">
         <v>551</v>
       </c>
@@ -5850,7 +5894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="75" t="s">
         <v>552</v>
       </c>
@@ -5861,7 +5905,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="409.5" customHeight="1">
+    <row r="36" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="75" t="s">
         <v>250</v>
       </c>
@@ -5872,7 +5916,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="409.5" customHeight="1">
+    <row r="37" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="75" t="s">
         <v>555</v>
       </c>
@@ -5883,7 +5927,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1">
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="75" t="s">
         <v>255</v>
       </c>
@@ -5894,7 +5938,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="242.25" customHeight="1">
+    <row r="39" spans="1:3" ht="242.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="75" t="s">
         <v>558</v>
       </c>
@@ -5905,7 +5949,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="140.25" customHeight="1">
+    <row r="40" spans="1:3" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="75" t="s">
         <v>253</v>
       </c>
@@ -5916,7 +5960,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="409.5" customHeight="1">
+    <row r="41" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="75" t="s">
         <v>561</v>
       </c>
@@ -5927,7 +5971,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="409.5" customHeight="1">
+    <row r="42" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="75" t="s">
         <v>533</v>
       </c>
@@ -5938,7 +5982,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="409.5" customHeight="1">
+    <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="75" t="s">
         <v>566</v>
       </c>
@@ -5949,7 +5993,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="409.5" customHeight="1">
+    <row r="44" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="75" t="s">
         <v>569</v>
       </c>
@@ -5960,7 +6004,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="178.5" customHeight="1">
+    <row r="45" spans="1:3" ht="178.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="75" t="s">
         <v>571</v>
       </c>
@@ -5971,7 +6015,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="409.5" customHeight="1">
+    <row r="46" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="75" t="s">
         <v>573</v>
       </c>
@@ -5982,7 +6026,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1">
+    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="75" t="s">
         <v>575</v>
       </c>
@@ -5993,7 +6037,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="76.5" customHeight="1">
+    <row r="48" spans="1:3" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="75" t="s">
         <v>576</v>
       </c>
@@ -6004,7 +6048,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1">
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="75" t="s">
         <v>579</v>
       </c>
@@ -6015,7 +6059,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1">
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="75" t="s">
         <v>580</v>
       </c>
@@ -6026,7 +6070,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="331.5" customHeight="1">
+    <row r="51" spans="1:3" ht="331.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="94" t="s">
         <v>581</v>
       </c>
@@ -6037,7 +6081,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1">
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="79" t="s">
         <v>583</v>
       </c>
@@ -6048,7 +6092,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1">
+    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="79" t="s">
         <v>254</v>
       </c>
@@ -6059,7 +6103,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1">
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="79" t="s">
         <v>584</v>
       </c>
@@ -6070,7 +6114,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="409.5" customHeight="1">
+    <row r="55" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="96" t="s">
         <v>586</v>
       </c>
@@ -6081,7 +6125,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="84" t="s">
         <v>588</v>
       </c>
@@ -6092,14 +6136,14 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="84" t="s">
         <v>589</v>
       </c>
       <c r="B57" s="93"/>
       <c r="C57" s="93"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="84" t="s">
         <v>590</v>
       </c>
@@ -6110,7 +6154,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="84" t="s">
         <v>591</v>
       </c>
@@ -6121,14 +6165,14 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="84" t="s">
         <v>592</v>
       </c>
       <c r="B60" s="97"/>
       <c r="C60" s="97"/>
     </row>
-    <row r="61" spans="1:3" ht="24.75">
+    <row r="61" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="84" t="s">
         <v>593</v>
       </c>
@@ -6139,7 +6183,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="178.5" customHeight="1">
+    <row r="62" spans="1:3" ht="178.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="84" t="s">
         <v>594</v>
       </c>
@@ -6150,7 +6194,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1">
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="99" t="s">
         <v>596</v>
       </c>
@@ -6161,7 +6205,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="24.75" customHeight="1">
+    <row r="64" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="99" t="s">
         <v>598</v>
       </c>
@@ -6172,7 +6216,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="24.75" customHeight="1">
+    <row r="65" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="99" t="s">
         <v>600</v>
       </c>
@@ -6183,7 +6227,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15" customHeight="1">
+    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="99" t="s">
         <v>602</v>
       </c>
@@ -6194,7 +6238,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="24.75" customHeight="1">
+    <row r="67" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="99" t="s">
         <v>604</v>
       </c>
@@ -6205,7 +6249,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15" customHeight="1">
+    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="99" t="s">
         <v>606</v>
       </c>
@@ -6216,7 +6260,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15" customHeight="1">
+    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="99" t="s">
         <v>569</v>
       </c>
@@ -6227,7 +6271,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15" customHeight="1">
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="99" t="s">
         <v>609</v>
       </c>
@@ -6238,7 +6282,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="25.5">
+    <row r="71" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" s="99" t="s">
         <v>561</v>
       </c>
@@ -6249,7 +6293,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="63.75">
+    <row r="72" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A72" s="99" t="s">
         <v>613</v>
       </c>
@@ -6261,8 +6305,10 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6274,13 +6320,13 @@
       <selection activeCell="A2" sqref="A2:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
@@ -6297,7 +6343,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>69</v>
       </c>
@@ -6311,7 +6357,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>11</v>
       </c>
@@ -6328,7 +6374,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>620</v>
       </c>
@@ -6342,7 +6388,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="108" t="s">
         <v>622</v>
       </c>
@@ -6356,7 +6402,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>51</v>
       </c>
@@ -6370,7 +6416,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>46</v>
       </c>
@@ -6384,7 +6430,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>51</v>
       </c>
@@ -6398,7 +6444,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="110" t="s">
         <v>56</v>
       </c>
@@ -6415,7 +6461,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>311</v>
       </c>
@@ -6429,7 +6475,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="108" t="s">
         <v>622</v>
       </c>
@@ -6443,7 +6489,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>327</v>
       </c>
@@ -6457,7 +6503,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>327</v>
       </c>
@@ -6471,7 +6517,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>623</v>
       </c>
@@ -6485,7 +6531,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="108" t="s">
         <v>622</v>
       </c>
@@ -6499,7 +6545,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="108" t="s">
         <v>622</v>
       </c>
@@ -6513,7 +6559,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="108" t="s">
         <v>624</v>
       </c>
@@ -6527,7 +6573,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="108" t="s">
         <v>431</v>
       </c>
@@ -6543,6 +6589,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E1"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6555,15 +6602,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B1" s="121" t="s">
         <v>665</v>
       </c>
@@ -6574,7 +6621,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="121" t="s">
         <v>0</v>
       </c>
@@ -6588,7 +6635,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A3" s="121" t="s">
         <v>119</v>
       </c>
@@ -6602,7 +6649,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A4" s="121" t="s">
         <v>667</v>
       </c>
@@ -6616,7 +6663,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="121" t="s">
         <v>668</v>
       </c>
@@ -6631,6 +6678,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6643,15 +6691,15 @@
       <selection sqref="A1:H98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="46" t="s">
         <v>374</v>
       </c>
@@ -6677,7 +6725,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="46" t="s">
         <v>380</v>
       </c>
@@ -6699,7 +6747,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="46" t="s">
         <v>380</v>
       </c>
@@ -6721,7 +6769,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="46" t="s">
         <v>380</v>
       </c>
@@ -6743,7 +6791,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="46" t="s">
         <v>380</v>
       </c>
@@ -6767,7 +6815,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="46" t="s">
         <v>380</v>
       </c>
@@ -6789,7 +6837,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="46" t="s">
         <v>380</v>
       </c>
@@ -6813,7 +6861,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="46" t="s">
         <v>380</v>
       </c>
@@ -6835,7 +6883,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="46" t="s">
         <v>380</v>
       </c>
@@ -6857,7 +6905,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="46" t="s">
         <v>380</v>
       </c>
@@ -6879,7 +6927,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="46" t="s">
         <v>393</v>
       </c>
@@ -6901,7 +6949,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="46" t="s">
         <v>393</v>
       </c>
@@ -6923,7 +6971,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="46" t="s">
         <v>393</v>
       </c>
@@ -6945,7 +6993,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="46" t="s">
         <v>395</v>
       </c>
@@ -6967,7 +7015,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="46" t="s">
         <v>397</v>
       </c>
@@ -6989,7 +7037,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="46" t="s">
         <v>399</v>
       </c>
@@ -7011,7 +7059,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="46" t="s">
         <v>399</v>
       </c>
@@ -7033,7 +7081,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>380</v>
       </c>
@@ -7057,7 +7105,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="46" t="s">
         <v>404</v>
       </c>
@@ -7079,7 +7127,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="46" t="s">
         <v>404</v>
       </c>
@@ -7101,7 +7149,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="46" t="s">
         <v>404</v>
       </c>
@@ -7123,7 +7171,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="46" t="s">
         <v>408</v>
       </c>
@@ -7145,7 +7193,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="48" t="s">
         <v>380</v>
       </c>
@@ -7167,7 +7215,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="48" t="s">
         <v>380</v>
       </c>
@@ -7189,7 +7237,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="48" t="s">
         <v>380</v>
       </c>
@@ -7211,7 +7259,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="48" t="s">
         <v>380</v>
       </c>
@@ -7233,7 +7281,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="48" t="s">
         <v>380</v>
       </c>
@@ -7255,7 +7303,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="48" t="s">
         <v>380</v>
       </c>
@@ -7277,7 +7325,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="48" t="s">
         <v>380</v>
       </c>
@@ -7301,7 +7349,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="48" t="s">
         <v>380</v>
       </c>
@@ -7325,7 +7373,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>380</v>
       </c>
@@ -7347,7 +7395,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1">
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>399</v>
       </c>
@@ -7369,7 +7417,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="48" t="s">
         <v>380</v>
       </c>
@@ -7391,7 +7439,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="48" t="s">
         <v>380</v>
       </c>
@@ -7413,7 +7461,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="48" t="s">
         <v>380</v>
       </c>
@@ -7437,7 +7485,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="48" t="s">
         <v>380</v>
       </c>
@@ -7459,7 +7507,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="48" t="s">
         <v>380</v>
       </c>
@@ -7481,7 +7529,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="48" t="s">
         <v>380</v>
       </c>
@@ -7503,7 +7551,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="48" t="s">
         <v>429</v>
       </c>
@@ -7525,7 +7573,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="48" t="s">
         <v>380</v>
       </c>
@@ -7547,7 +7595,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="48" t="s">
         <v>380</v>
       </c>
@@ -7569,7 +7617,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A42" s="48" t="s">
         <v>380</v>
       </c>
@@ -7591,7 +7639,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A43" s="48" t="s">
         <v>380</v>
       </c>
@@ -7613,7 +7661,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A44" s="48" t="s">
         <v>380</v>
       </c>
@@ -7635,7 +7683,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.15">
       <c r="A45" s="48" t="s">
         <v>380</v>
       </c>
@@ -7657,7 +7705,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1">
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
         <v>434</v>
       </c>
@@ -7679,7 +7727,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1">
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
         <v>434</v>
       </c>
@@ -7701,7 +7749,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" thickBot="1">
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
         <v>434</v>
       </c>
@@ -7723,7 +7771,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75" thickBot="1">
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
         <v>434</v>
       </c>
@@ -7745,7 +7793,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1">
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>434</v>
       </c>
@@ -7767,7 +7815,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" thickBot="1">
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
         <v>434</v>
       </c>
@@ -7789,7 +7837,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1">
+    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
         <v>380</v>
       </c>
@@ -7811,7 +7859,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1">
+    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
         <v>380</v>
       </c>
@@ -7833,7 +7881,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15.75" thickBot="1">
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
         <v>380</v>
       </c>
@@ -7855,7 +7903,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1">
+    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
         <v>434</v>
       </c>
@@ -7877,7 +7925,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1">
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
         <v>434</v>
       </c>
@@ -7899,7 +7947,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75" thickBot="1">
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
         <v>380</v>
       </c>
@@ -7921,7 +7969,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.75" thickBot="1">
+    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
         <v>444</v>
       </c>
@@ -7943,7 +7991,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.75" thickBot="1">
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
         <v>444</v>
       </c>
@@ -7965,7 +8013,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15.75" thickBot="1">
+    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
         <v>447</v>
       </c>
@@ -7987,7 +8035,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" thickBot="1">
+    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="18" t="s">
         <v>447</v>
       </c>
@@ -8009,7 +8057,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>628</v>
       </c>
@@ -8029,7 +8077,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>628</v>
       </c>
@@ -8049,7 +8097,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>633</v>
       </c>
@@ -8069,7 +8117,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>628</v>
       </c>
@@ -8089,7 +8137,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>628</v>
       </c>
@@ -8109,7 +8157,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>633</v>
       </c>
@@ -8129,7 +8177,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>633</v>
       </c>
@@ -8149,7 +8197,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>628</v>
       </c>
@@ -8169,7 +8217,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>638</v>
       </c>
@@ -8189,7 +8237,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>638</v>
       </c>
@@ -8209,7 +8257,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>628</v>
       </c>
@@ -8229,7 +8277,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>628</v>
       </c>
@@ -8249,7 +8297,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>628</v>
       </c>
@@ -8269,7 +8317,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>628</v>
       </c>
@@ -8289,7 +8337,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>633</v>
       </c>
@@ -8309,7 +8357,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>633</v>
       </c>
@@ -8329,7 +8377,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>633</v>
       </c>
@@ -8349,7 +8397,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>633</v>
       </c>
@@ -8369,7 +8417,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>633</v>
       </c>
@@ -8389,7 +8437,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>633</v>
       </c>
@@ -8409,7 +8457,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>633</v>
       </c>
@@ -8429,7 +8477,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>628</v>
       </c>
@@ -8449,7 +8497,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>628</v>
       </c>
@@ -8469,7 +8517,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>633</v>
       </c>
@@ -8489,7 +8537,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>633</v>
       </c>
@@ -8509,7 +8557,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>628</v>
       </c>
@@ -8529,7 +8577,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>633</v>
       </c>
@@ -8549,7 +8597,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>633</v>
       </c>
@@ -8569,7 +8617,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>633</v>
       </c>
@@ -8589,7 +8637,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>633</v>
       </c>
@@ -8609,7 +8657,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>633</v>
       </c>
@@ -8629,7 +8677,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>633</v>
       </c>
@@ -8649,7 +8697,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>633</v>
       </c>
@@ -8669,7 +8717,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>633</v>
       </c>
@@ -8689,7 +8737,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>633</v>
       </c>
@@ -8709,7 +8757,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>633</v>
       </c>
@@ -8729,7 +8777,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>633</v>
       </c>
@@ -8763,16 +8811,16 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8801,7 +8849,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>125</v>
       </c>
@@ -8830,7 +8878,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>199</v>
       </c>
@@ -8859,7 +8907,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>202</v>
       </c>
@@ -8888,7 +8936,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>207</v>
       </c>
@@ -8917,7 +8965,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>135</v>
       </c>
@@ -8944,7 +8992,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>211</v>
       </c>
@@ -8973,7 +9021,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>212</v>
       </c>
@@ -9002,7 +9050,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>140</v>
       </c>
@@ -9031,7 +9079,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>105</v>
       </c>
@@ -9060,7 +9108,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>103</v>
       </c>
@@ -9089,7 +9137,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>218</v>
       </c>
@@ -9118,7 +9166,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.5" customHeight="1" thickBot="1">
+    <row r="13" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>218</v>
       </c>
@@ -9172,17 +9220,17 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>144</v>
       </c>
@@ -9205,7 +9253,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -9228,7 +9276,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -9251,7 +9299,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -9274,7 +9322,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -9297,7 +9345,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -9320,7 +9368,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -9343,7 +9391,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
@@ -9366,7 +9414,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>97</v>
       </c>
@@ -9389,7 +9437,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>24</v>
       </c>
@@ -9406,7 +9454,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
@@ -9425,7 +9473,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>97</v>
       </c>
@@ -9462,18 +9510,18 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>182</v>
       </c>
@@ -9499,7 +9547,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>61</v>
       </c>
@@ -9525,7 +9573,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>188</v>
       </c>
@@ -9551,7 +9599,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
@@ -9577,7 +9625,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>32</v>
       </c>
@@ -9603,7 +9651,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>195</v>
       </c>
@@ -9676,12 +9724,12 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45.75" thickBot="1">
+    <row r="1" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>222</v>
       </c>
@@ -9707,7 +9755,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -9733,7 +9781,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -9759,7 +9807,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28">
         <v>7</v>
       </c>
@@ -9804,15 +9852,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="4" max="4" width="41.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>236</v>
       </c>
@@ -9826,7 +9874,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60">
+    <row r="2" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A2" s="31" t="s">
         <v>676</v>
       </c>
@@ -9840,7 +9888,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="105">
+    <row r="3" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
         <v>238</v>
       </c>
@@ -9854,7 +9902,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
         <v>240</v>
       </c>
@@ -9866,7 +9914,7 @@
       </c>
       <c r="D4" s="32"/>
     </row>
-    <row r="5" spans="1:4" ht="60">
+    <row r="5" spans="1:4" ht="54" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>243</v>
       </c>
@@ -9880,7 +9928,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>246</v>
       </c>
@@ -9892,7 +9940,7 @@
       </c>
       <c r="D6" s="32"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
         <v>247</v>
       </c>
@@ -9904,7 +9952,7 @@
       </c>
       <c r="D7" s="32"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="31" t="s">
         <v>250</v>
       </c>
@@ -9916,7 +9964,7 @@
       </c>
       <c r="D8" s="32"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
         <v>253</v>
       </c>
@@ -9924,7 +9972,7 @@
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
         <v>254</v>
       </c>
@@ -9932,7 +9980,7 @@
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
         <v>255</v>
       </c>
@@ -9944,7 +9992,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="36" t="s">
         <v>247</v>
       </c>
@@ -9970,16 +10018,16 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="134.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>236</v>
       </c>
@@ -9996,7 +10044,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>260</v>
       </c>
@@ -10010,7 +10058,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -10024,7 +10072,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>265</v>
       </c>
@@ -10041,7 +10089,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -10052,7 +10100,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>270</v>
       </c>
@@ -10060,7 +10108,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>272</v>
       </c>
@@ -10068,7 +10116,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>274</v>
       </c>
@@ -10076,7 +10124,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>276</v>
       </c>
@@ -10104,15 +10152,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>182</v>
       </c>
@@ -10126,7 +10174,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>32</v>
       </c>
@@ -10140,7 +10188,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
         <v>71</v>
       </c>
@@ -10154,7 +10202,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>75</v>
       </c>
@@ -10168,7 +10216,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
         <v>24</v>
       </c>
@@ -10180,7 +10228,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>18</v>
       </c>
@@ -10192,7 +10240,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>23</v>
       </c>
@@ -10204,7 +10252,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
         <v>79</v>
       </c>
@@ -10218,7 +10266,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
         <v>36</v>
       </c>
@@ -10230,7 +10278,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="42" t="s">
         <v>42</v>
       </c>
@@ -10242,7 +10290,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
         <v>47</v>
       </c>
@@ -10254,7 +10302,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
         <v>52</v>
       </c>
@@ -10266,7 +10314,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
         <v>57</v>
       </c>
@@ -10280,7 +10328,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
         <v>61</v>
       </c>
@@ -10292,7 +10340,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="42" t="s">
         <v>65</v>
       </c>
@@ -10304,7 +10352,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="42" t="s">
         <v>70</v>
       </c>

</xml_diff>